<commit_message>
Add `predicate` slot to `SynonymPredicateChange`
</commit_message>
<xml_diff>
--- a/project/excel/kgcl.xlsx
+++ b/project/excel/kgcl.xlsx
@@ -2938,7 +2938,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2964,90 +2964,95 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>predicate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>about_node</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>about_node_representation</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>language</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>old_value_type</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>new_value_type</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>new_language</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>old_language</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>new_datatype</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>old_datatype</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>was_generated_by</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>pull_request</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_undo</t>
         </is>

</xml_diff>

<commit_message>
Add predicate slot to NewSynonym
</commit_message>
<xml_diff>
--- a/project/excel/kgcl.xlsx
+++ b/project/excel/kgcl.xlsx
@@ -2444,7 +2444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2470,90 +2470,95 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>predicate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>about_node</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>about_node_representation</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>old_value</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>old_value_type</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>new_value_type</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>new_language</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>old_language</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>new_datatype</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>old_datatype</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>was_generated_by</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>pull_request</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_undo</t>
         </is>

</xml_diff>

<commit_message>
Rebuild project artifacts (#93)
</commit_message>
<xml_diff>
--- a/project/excel/kgcl.xlsx
+++ b/project/excel/kgcl.xlsx
@@ -588,7 +588,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,22 +629,37 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -659,7 +674,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,22 +715,37 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -748,14 +778,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>about</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_undo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>old_value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>new_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -766,14 +819,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>about</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_undo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>old_value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>new_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -784,7 +860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -910,22 +986,42 @@
       </c>
       <c r="X1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -940,7 +1036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1066,22 +1162,42 @@
       </c>
       <c r="X1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,22 +1338,42 @@
       </c>
       <c r="X1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1409,22 +1545,42 @@
       </c>
       <c r="X1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -1439,7 +1595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1555,22 +1711,42 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1681,22 +1857,37 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -1711,7 +1902,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1837,22 +2028,42 @@
       </c>
       <c r="X1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -1867,7 +2078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1973,22 +2184,37 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -2003,7 +2229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2109,22 +2335,37 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2245,22 +2486,37 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -2275,7 +2531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2371,22 +2627,37 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -2401,7 +2672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2497,22 +2768,37 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -2527,7 +2813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2603,22 +2889,37 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2775,22 +3076,37 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -2805,7 +3121,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2896,22 +3212,42 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -2926,7 +3262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3027,22 +3363,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3408,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3158,22 +3509,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3188,7 +3554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3279,22 +3645,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3309,7 +3690,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3410,22 +3791,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3440,7 +3836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3531,22 +3927,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3561,7 +3972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3652,22 +4063,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3682,7 +4108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3783,22 +4209,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3813,7 +4254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3914,22 +4355,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -3990,7 +4446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4081,22 +4537,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4111,7 +4582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4212,22 +4683,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4242,7 +4728,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4343,22 +4829,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4373,7 +4874,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4464,22 +4965,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4494,7 +5010,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4585,22 +5101,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4615,7 +5146,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4706,22 +5237,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4736,7 +5282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4837,22 +5383,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4867,7 +5428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4968,22 +5529,37 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -4998,7 +5574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5089,22 +5665,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -5119,7 +5710,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5210,22 +5801,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -5286,7 +5892,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5377,22 +5983,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -5407,7 +6028,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5498,22 +6119,37 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
         </is>
       </c>
     </row>
@@ -5523,636 +6159,6 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>old_value</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>new_value</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_textual_diff</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>about_node</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>about_node_representation</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>old_value_type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>new_value_type</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>new_language</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>old_language</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>new_datatype</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>old_datatype</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>pull_request</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>change_date</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>contributor</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_undo</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>about_node</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>about_node_representation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>old_value</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>new_value</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>old_value_type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>new_value_type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>new_language</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>old_language</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>new_datatype</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>old_datatype</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>pull_request</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>change_date</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>contributor</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_undo</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>about_node</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>about_node_representation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>old_value</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>new_value</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>old_value_type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>new_value_type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>new_language</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>old_language</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>new_datatype</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>old_datatype</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>pull_request</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>change_date</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>contributor</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_undo</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_direct_replacement</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_nondirect_replacement</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>about_node</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>about_node_representation</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>old_value</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>new_value</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>old_value_type</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>new_value_type</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>new_language</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>old_language</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>new_datatype</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>old_datatype</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>pull_request</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>change_date</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>contributor</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>has_undo</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>about_node</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>about_node_representation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>old_value</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>new_value</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>old_value_type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>new_value_type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>new_language</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>old_language</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>new_datatype</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>old_datatype</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>pull_request</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>change_date</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>contributor</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_undo</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6169,6 +6175,741 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>old_value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>new_value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_textual_diff</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>about_node</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>about_node_representation</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>old_value_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>new_value_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>new_language</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>old_language</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>new_datatype</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>old_datatype</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>was_generated_by</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>pull_request</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>change_date</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>has_undo</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Y1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>about_node</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>about_node_representation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>old_value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>new_value</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>old_value_type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>new_value_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>new_language</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>old_language</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>new_datatype</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>old_datatype</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>was_generated_by</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>pull_request</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>change_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>about</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Y1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>about_node</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>about_node_representation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>old_value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>new_value</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>old_value_type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>new_value_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>new_language</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>old_language</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>new_datatype</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>old_datatype</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>was_generated_by</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>pull_request</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>change_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>about</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_direct_replacement</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_nondirect_replacement</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>about_node</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>about_node_representation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>old_value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>new_value</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>old_value_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>new_value_type</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>new_language</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>old_language</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>new_datatype</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>old_datatype</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>was_generated_by</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>pull_request</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>change_date</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>about</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_direct_replacement</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_nondirect_replacement</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>about_node</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>about_node_representation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>old_value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>new_value</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>old_value_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>new_value_type</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>new_language</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>old_language</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>new_datatype</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>old_datatype</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>was_generated_by</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>pull_request</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>change_date</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>about</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AB1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>node_id</t>
         </is>
       </c>
@@ -6269,22 +7010,42 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -6304,7 +7065,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6420,22 +7181,42 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -6455,7 +7236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6566,22 +7347,42 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -6647,7 +7448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6738,22 +7539,42 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -6768,7 +7589,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6869,22 +7690,42 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -6899,7 +7740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7000,22 +7841,42 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>
@@ -7030,7 +7891,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7131,22 +7992,42 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>term_tracker_issue</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>change_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>contributor</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>has_undo</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>change_description</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>associated_change_set</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>about</t>
         </is>
       </c>
     </row>

</xml_diff>